<commit_message>
Upsert with excel sheet implementation
</commit_message>
<xml_diff>
--- a/src/main/resources/transactions.xlsx
+++ b/src/main/resources/transactions.xlsx
@@ -2,16 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>description</t>
   </si>
@@ -29,6 +31,12 @@
   </si>
   <si>
     <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -286,52 +294,68 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" customWidth="false" hidden="true" width="8.0"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" t="s" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" t="n" s="1">
         <v>1900.0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" t="n" s="2">
         <v>45839.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="1">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" t="n" s="1">
         <v>500.05</v>
       </c>
-      <c r="C3" s="2">
-        <v>45840.0</v>
+      <c r="D3" t="n" s="2">
+        <v>45841.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="1">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" t="n" s="1">
         <v>650.0</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" t="n" s="2">
         <v>45841.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel importing + exporting work
</commit_message>
<xml_diff>
--- a/src/main/resources/transactions.xlsx
+++ b/src/main/resources/transactions.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
   <si>
     <t>description</t>
   </si>
@@ -37,6 +37,27 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2025-07-01</t>
+  </si>
+  <si>
+    <t>2025-07-03</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>2025-07-10</t>
   </si>
 </sst>
 </file>
@@ -301,62 +322,65 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" customWidth="false" hidden="true" width="8.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5390625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.515625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0390625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B1" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>2</v>
+      <c r="B1" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
         <v>1.0</v>
       </c>
-      <c r="B2" t="s" s="1">
+      <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="C2" t="n" s="1">
+      <c r="C2" t="n" s="0">
         <v>1900.0</v>
       </c>
-      <c r="D2" t="n" s="2">
-        <v>45839.0</v>
+      <c r="D2" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s" s="1">
-        <v>4</v>
-      </c>
-      <c r="C3" t="n" s="1">
-        <v>500.05</v>
-      </c>
-      <c r="D3" t="n" s="2">
-        <v>45841.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>650.0</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n" s="1">
-        <v>650.0</v>
-      </c>
-      <c r="D4" t="n" s="2">
-        <v>45841.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>1300.0</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented recipient and payment services and fixed sync issues
</commit_message>
<xml_diff>
--- a/src/main/resources/transactions.xlsx
+++ b/src/main/resources/transactions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -46,31 +46,22 @@
     <t xml:space="preserve">2025-07-12</t>
   </si>
   <si>
-    <t xml:space="preserve">Storage Unit</t>
-  </si>
-  <si>
     <t xml:space="preserve">PS5</t>
   </si>
   <si>
     <t xml:space="preserve">2025-07-16</t>
   </si>
   <si>
-    <t xml:space="preserve">Rolex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-01-01</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nintendo Switch 2</t>
   </si>
   <si>
     <t xml:space="preserve">2025-06-02</t>
   </si>
   <si>
-    <t xml:space="preserve">Birthday Gift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-03-27</t>
+    <t xml:space="preserve">Payment to Shreyansh Kaushik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-21</t>
   </si>
 </sst>
 </file>
@@ -349,18 +340,18 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048575"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="true" style="1" width="8.0" collapsed="false" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="15.43" collapsed="false" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="7.51" collapsed="false" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="10.04" collapsed="false" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="1" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,61 +398,48 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>65</v>
+        <v>799.99</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>799.99</v>
+        <v>550</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>50000</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>550</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>